<commit_message>
Fix bugs, db first version + refactoring
</commit_message>
<xml_diff>
--- a/GoldReserves.Backend/world_official_gold_holdings_as_of_april2016_ifs.xlsx
+++ b/GoldReserves.Backend/world_official_gold_holdings_as_of_april2016_ifs.xlsx
@@ -22,7 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">PDF!$A$1:$H$145</definedName>
     <definedName name="right" localSheetId="0">PDF!$F$8:$H$58</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1550,8 +1550,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A3:N146"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A35" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1630,7 +1630,7 @@
         <v>77</v>
       </c>
       <c r="C7" s="8">
-        <v>2</v>
+        <v>8133.4616724207644</v>
       </c>
       <c r="D7" s="9">
         <v>0.75256008711692501</v>
@@ -1656,7 +1656,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="8">
-        <v>3380.9834841840102</v>
+        <v>3380.9834841840066</v>
       </c>
       <c r="D8" s="9">
         <v>0.69003165583922066</v>
@@ -1734,7 +1734,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="8">
-        <v>2435.6318621504802</v>
+        <v>2435.6318621504774</v>
       </c>
       <c r="D11" s="9">
         <v>0.63177404607096543</v>
@@ -3875,15 +3875,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B32AA5C-29E8-4E90-8254-F0634DECBFA8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="2bbd67e2-e8b5-429c-83f4-c3205d8c9d1c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>